<commit_message>
Loan and Deposit Balance Report
- Include Credit officer on Loan Accounts and Deposit Accounts reports
</commit_message>
<xml_diff>
--- a/public/templates/Reports/Deposit Accounts.xlsx
+++ b/public/templates/Reports/Deposit Accounts.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashbeemorgado/devs/lumen/public/templates/Reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nelsontan/Projects/Lumen/public/templates/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D3B01C-3402-A041-B683-CCF1A6CF442A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288A6496-083C-A443-ACC7-C840EEF67F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>#</t>
   </si>
@@ -44,6 +54,9 @@
   </si>
   <si>
     <t>ACCRUED INTEREST</t>
+  </si>
+  <si>
+    <t>LOAN OFFICER</t>
   </si>
 </sst>
 </file>
@@ -411,26 +424,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H2"/>
+  <dimension ref="A2:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" customWidth="1"/>
-    <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="36.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,21 +451,24 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>